<commit_message>
major changes for new release
</commit_message>
<xml_diff>
--- a/data/wgi_governance_scores_2023_with_iso3.xlsx
+++ b/data/wgi_governance_scores_2023_with_iso3.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\FLIM\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3EBDC6-E1FA-43EF-9136-4CE9181A02F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
-  <si>
-    <t>iso3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="429">
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>governance_score</t>
+  </si>
+  <si>
+    <t>ISO</t>
   </si>
   <si>
     <t>Afghanistan</t>
@@ -706,6 +706,9 @@
     <t>AZE</t>
   </si>
   <si>
+    <t>BHS</t>
+  </si>
+  <si>
     <t>BHR</t>
   </si>
   <si>
@@ -766,6 +769,9 @@
     <t>CAN</t>
   </si>
   <si>
+    <t>CPV</t>
+  </si>
+  <si>
     <t>CYM</t>
   </si>
   <si>
@@ -787,6 +793,12 @@
     <t>COM</t>
   </si>
   <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>COG</t>
+  </si>
+  <si>
     <t>COK</t>
   </si>
   <si>
@@ -823,6 +835,9 @@
     <t>ECU</t>
   </si>
   <si>
+    <t>EGY</t>
+  </si>
+  <si>
     <t>SLV</t>
   </si>
   <si>
@@ -856,6 +871,9 @@
     <t>GAB</t>
   </si>
   <si>
+    <t>GMB</t>
+  </si>
+  <si>
     <t>GEO</t>
   </si>
   <si>
@@ -895,6 +913,9 @@
     <t>HND</t>
   </si>
   <si>
+    <t>HKG</t>
+  </si>
+  <si>
     <t>HUN</t>
   </si>
   <si>
@@ -907,6 +928,9 @@
     <t>IDN</t>
   </si>
   <si>
+    <t>IRN</t>
+  </si>
+  <si>
     <t>IRQ</t>
   </si>
   <si>
@@ -925,6 +949,9 @@
     <t>JPN</t>
   </si>
   <si>
+    <t>JEY</t>
+  </si>
+  <si>
     <t>JOR</t>
   </si>
   <si>
@@ -937,12 +964,24 @@
     <t>KIR</t>
   </si>
   <si>
+    <t>PRK</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
+    <t>XKX</t>
+  </si>
+  <si>
     <t>KWT</t>
   </si>
   <si>
     <t>KGZ</t>
   </si>
   <si>
+    <t>LAO</t>
+  </si>
+  <si>
     <t>LVA</t>
   </si>
   <si>
@@ -967,6 +1006,9 @@
     <t>LUX</t>
   </si>
   <si>
+    <t>MAC</t>
+  </si>
+  <si>
     <t>MDG</t>
   </si>
   <si>
@@ -1000,6 +1042,9 @@
     <t>MEX</t>
   </si>
   <si>
+    <t>FSM</t>
+  </si>
+  <si>
     <t>MDA</t>
   </si>
   <si>
@@ -1150,6 +1195,15 @@
     <t>LKA</t>
   </si>
   <si>
+    <t>KNA</t>
+  </si>
+  <si>
+    <t>LCA</t>
+  </si>
+  <si>
+    <t>VCT</t>
+  </si>
+  <si>
     <t>SDN</t>
   </si>
   <si>
@@ -1165,6 +1219,12 @@
     <t>SYR</t>
   </si>
   <si>
+    <t>STP</t>
+  </si>
+  <si>
+    <t>TWN</t>
+  </si>
+  <si>
     <t>TJK</t>
   </si>
   <si>
@@ -1195,6 +1255,9 @@
     <t>TUV</t>
   </si>
   <si>
+    <t>TUR</t>
+  </si>
+  <si>
     <t>UGA</t>
   </si>
   <si>
@@ -1219,26 +1282,32 @@
     <t>VUT</t>
   </si>
   <si>
+    <t>VEN</t>
+  </si>
+  <si>
     <t>VNM</t>
   </si>
   <si>
+    <t>VIR</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>YEM</t>
+  </si>
+  <si>
     <t>ZMB</t>
   </si>
   <si>
     <t>ZWE</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>governance_score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,21 +1370,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1353,7 +1414,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1387,7 +1448,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1422,10 +1482,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1598,2292 +1657,2365 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>402</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>403</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0.1970994174480438</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>0.49632465615868571</v>
+        <v>0.4963246561586857</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>0.35570524930953978</v>
+        <v>0.3557052493095398</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>0.68150143027305599</v>
+        <v>0.681501430273056</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>0.77771197557449345</v>
+        <v>0.7777119755744935</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>0.32603580057621012</v>
+        <v>0.3260358005762101</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>0.70339966118335728</v>
+        <v>0.7033996611833573</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>0.58159167319536209</v>
+        <v>0.5815916731953621</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>0.41841183900833129</v>
+        <v>0.4184118390083313</v>
       </c>
       <c r="C10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>0.48999433591961861</v>
+        <v>0.4899943359196186</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>0.68606646656990056</v>
+        <v>0.6860664665699006</v>
       </c>
       <c r="C12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>0.84182370305061338</v>
+        <v>0.8418237030506134</v>
       </c>
       <c r="C13" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>0.77841349840164187</v>
+        <v>0.7784134984016419</v>
       </c>
       <c r="C14" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>0.40482453648000949</v>
+        <v>0.4048245364800095</v>
       </c>
       <c r="C15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0.5862006809329614</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>0.62108696475625036</v>
+        <v>0.6210869647562504</v>
       </c>
       <c r="C17" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>0.33824946284294127</v>
+        <v>0.3382494628429413</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>0.63211661279201503</v>
+        <v>0.632116612792015</v>
       </c>
       <c r="C19" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>0.28365150094032288</v>
+        <v>0.2836515009403229</v>
       </c>
       <c r="C20" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>0.74187330603599544</v>
+        <v>0.7418733060359954</v>
       </c>
       <c r="C21" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>0.41656898334622378</v>
+        <v>0.4165689833462238</v>
       </c>
       <c r="C22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>0.44649452380836008</v>
+        <v>0.4464945238083601</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>0.70339966118335728</v>
+        <v>0.7033996611833573</v>
       </c>
       <c r="C24" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>0.6182195246219635</v>
       </c>
       <c r="C25" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>0.30628805756568911</v>
+        <v>0.3062880575656891</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>0.39787583947181698</v>
+        <v>0.397875839471817</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>0.60022458434104919</v>
+        <v>0.6002245843410492</v>
       </c>
       <c r="C28" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>0.4172155737876892</v>
       </c>
       <c r="C29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>0.72717843055725095</v>
+        <v>0.727178430557251</v>
       </c>
       <c r="C30" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>0.51552147052716468</v>
+        <v>0.5155214705271647</v>
       </c>
       <c r="C31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32">
-        <v>0.38883722424507139</v>
+        <v>0.3888372242450714</v>
       </c>
       <c r="C32" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>0.25035370588302608</v>
+        <v>0.2503537058830261</v>
       </c>
       <c r="C33" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>0.34455815553665159</v>
+        <v>0.3445581555366516</v>
       </c>
       <c r="C34" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>0.29897533953189848</v>
+        <v>0.2989753395318985</v>
       </c>
       <c r="C35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>0.81530101895332341</v>
+        <v>0.8153010189533234</v>
       </c>
       <c r="C36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B37">
-        <v>0.58207710715942085</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5820771071594208</v>
+      </c>
+      <c r="C37" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B38">
-        <v>0.67316876798868175</v>
+        <v>0.6731687679886817</v>
       </c>
       <c r="C38" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B39">
-        <v>0.18628407120704649</v>
+        <v>0.1862840712070465</v>
       </c>
       <c r="C39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>0.226389217376709</v>
       </c>
       <c r="C40" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41">
-        <v>0.66184925138950346</v>
+        <v>0.6618492513895035</v>
       </c>
       <c r="C41" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B42">
-        <v>0.51385030718520286</v>
+        <v>0.5138503071852029</v>
       </c>
       <c r="C42" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43">
-        <v>0.46288460642099383</v>
+        <v>0.4628846064209938</v>
       </c>
       <c r="C43" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>0.2447535663843155</v>
       </c>
       <c r="C44" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>0.1875554978847504</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46">
-        <v>0.25302200317382822</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.2530220031738282</v>
+      </c>
+      <c r="C46" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47">
-        <v>0.46315536759793757</v>
+        <v>0.4631553675979376</v>
       </c>
       <c r="C47" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>0.59234050512313841</v>
+        <v>0.5923405051231384</v>
       </c>
       <c r="C48" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49">
-        <v>0.59495441094040868</v>
+        <v>0.5949544109404087</v>
       </c>
       <c r="C49" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50">
-        <v>0.37574900761246682</v>
+        <v>0.3757490076124668</v>
       </c>
       <c r="C50" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>0.62383729517459874</v>
+        <v>0.6238372951745987</v>
       </c>
       <c r="C51" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52">
-        <v>0.71642467379570007</v>
+        <v>0.7164246737957001</v>
       </c>
       <c r="C52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>0.43751010186970241</v>
+        <v>0.4375101018697024</v>
       </c>
       <c r="C53" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>0.907007884979248</v>
       </c>
       <c r="C54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>0.32146879732608802</v>
+        <v>0.321468797326088</v>
       </c>
       <c r="C55" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>0.58692224025726314</v>
+        <v>0.5869222402572631</v>
       </c>
       <c r="C56" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>0.48605770543217658</v>
+        <v>0.4860577054321766</v>
       </c>
       <c r="C57" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>0.35912128984928132</v>
+        <v>0.3591212898492813</v>
       </c>
       <c r="C58" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>0.4081528954207897</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>0.4405930619686842</v>
       </c>
       <c r="C60" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>0.2148082911968231</v>
       </c>
       <c r="C61" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B62">
-        <v>0.13029651045799259</v>
+        <v>0.1302965104579926</v>
       </c>
       <c r="C62" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B63">
-        <v>0.78288123607635496</v>
+        <v>0.782881236076355</v>
       </c>
       <c r="C63" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B64">
-        <v>0.35324191153049472</v>
+        <v>0.3532419115304947</v>
       </c>
       <c r="C64" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65">
-        <v>0.35374967902898791</v>
+        <v>0.3537496790289879</v>
       </c>
       <c r="C65" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B66">
-        <v>0.56058657802641387</v>
+        <v>0.5605865780264139</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B67">
-        <v>0.88461592197418215</v>
+        <v>0.8846159219741822</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B68">
-        <v>0.73317621946334843</v>
+        <v>0.7331762194633484</v>
       </c>
       <c r="C68" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B69">
-        <v>0.72080518901348112</v>
+        <v>0.7208051890134811</v>
       </c>
       <c r="C69" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>0.33135746717453002</v>
+        <v>0.33135746717453</v>
       </c>
       <c r="C70" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B71">
-        <v>0.40571872293949129</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.4057187229394913</v>
+      </c>
+      <c r="C71" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B72">
-        <v>0.62664190754294391</v>
+        <v>0.6266419075429439</v>
       </c>
       <c r="C72" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B73">
-        <v>0.79288828372955322</v>
+        <v>0.7928882837295532</v>
       </c>
       <c r="C73" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B74">
-        <v>0.47640136033296587</v>
+        <v>0.4764013603329659</v>
       </c>
       <c r="C74" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B75">
-        <v>0.55189719274640081</v>
+        <v>0.5518971927464008</v>
       </c>
       <c r="C75" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B76">
         <v>0.7341701924800873</v>
       </c>
       <c r="C76" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B77">
-        <v>0.57358777914196257</v>
+        <v>0.5735877791419626</v>
       </c>
       <c r="C77" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B78">
-        <v>0.66828103959560403</v>
+        <v>0.668281039595604</v>
       </c>
       <c r="C78" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B79">
-        <v>0.33077939003705981</v>
+        <v>0.3307793900370598</v>
       </c>
       <c r="C79" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80">
-        <v>0.30021822154521938</v>
+        <v>0.3002182215452194</v>
       </c>
       <c r="C80" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B81">
-        <v>0.23513668775558469</v>
+        <v>0.2351366877555847</v>
       </c>
       <c r="C81" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>0.42082486003637309</v>
+        <v>0.4208248600363731</v>
       </c>
       <c r="C82" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B83">
         <v>0.1788291335105896</v>
       </c>
       <c r="C83" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B84">
-        <v>0.32234620153903959</v>
+        <v>0.3223462015390396</v>
       </c>
       <c r="C84" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B85">
-        <v>0.80389793515205388</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.8038979351520539</v>
+      </c>
+      <c r="C85" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B86">
-        <v>0.55588273332978133</v>
+        <v>0.5558827333297813</v>
       </c>
       <c r="C86" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B87">
-        <v>0.80559942722320554</v>
+        <v>0.8055994272232055</v>
       </c>
       <c r="C87" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>0.5080245189368725</v>
       </c>
       <c r="C88" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>0.5120614238083363</v>
       </c>
       <c r="C89" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B90">
-        <v>0.24986420869827269</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.2498642086982727</v>
+      </c>
+      <c r="C90" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B91">
-        <v>0.20789309740066531</v>
+        <v>0.2078930974006653</v>
       </c>
       <c r="C91" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B92">
-        <v>0.82746909260749812</v>
+        <v>0.8274690926074981</v>
       </c>
       <c r="C92" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B93">
-        <v>0.69401867687702179</v>
+        <v>0.6940186768770218</v>
       </c>
       <c r="C93" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B94">
-        <v>0.60977782607078557</v>
+        <v>0.6097778260707856</v>
       </c>
       <c r="C94" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B95">
-        <v>0.51093621663749222</v>
+        <v>0.5109362166374922</v>
       </c>
       <c r="C95" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B96">
-        <v>0.80158954858779907</v>
+        <v>0.8015895485877991</v>
       </c>
       <c r="C96" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B97">
-        <v>0.74380027055740361</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7438002705574036</v>
+      </c>
+      <c r="C97" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B98">
-        <v>0.54751728922128673</v>
+        <v>0.5475172892212867</v>
       </c>
       <c r="C98" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B99">
-        <v>0.47496973834931849</v>
+        <v>0.4749697383493185</v>
       </c>
       <c r="C99" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B100">
-        <v>0.41042267829179763</v>
+        <v>0.4104226782917976</v>
       </c>
       <c r="C100" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B101">
-        <v>0.53121258951723571</v>
+        <v>0.5312125895172357</v>
       </c>
       <c r="C101" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B102">
-        <v>0.14511125683784479</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.1451112568378448</v>
+      </c>
+      <c r="C102" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B103">
-        <v>0.73349606692790981</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7334960669279098</v>
+      </c>
+      <c r="C103" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B104">
         <v>0.4563917011022568</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B105">
-        <v>0.54383710622787473</v>
+        <v>0.5438371062278747</v>
       </c>
       <c r="C105" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B106">
-        <v>0.30486669838428498</v>
+        <v>0.304866698384285</v>
       </c>
       <c r="C106" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B107">
-        <v>0.33110907971858983</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.3311090797185898</v>
+      </c>
+      <c r="C107" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B108">
-        <v>0.68033792674541482</v>
+        <v>0.6803379267454148</v>
       </c>
       <c r="C108" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B109">
-        <v>0.25065094232559199</v>
+        <v>0.250650942325592</v>
       </c>
       <c r="C109" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B110">
-        <v>0.37333742678165438</v>
+        <v>0.3733374267816544</v>
       </c>
       <c r="C110" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B111">
-        <v>0.29004778861999508</v>
+        <v>0.2900477886199951</v>
       </c>
       <c r="C111" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B112">
-        <v>0.15616988539695739</v>
+        <v>0.1561698853969574</v>
       </c>
       <c r="C112" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B113">
-        <v>0.83359481692314152</v>
+        <v>0.8335948169231415</v>
       </c>
       <c r="C113" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B114">
-        <v>0.72184525132179256</v>
+        <v>0.7218452513217926</v>
       </c>
       <c r="C114" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B115">
-        <v>0.87611851692199705</v>
+        <v>0.876118516921997</v>
       </c>
       <c r="C115" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B116">
-        <v>0.72582591176033018</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7258259117603302</v>
+      </c>
+      <c r="C116" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B117">
         <v>0.310127454996109</v>
       </c>
       <c r="C117" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B118">
-        <v>0.38049379065632821</v>
+        <v>0.3804937906563282</v>
       </c>
       <c r="C118" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B119">
-        <v>0.62019003778696058</v>
+        <v>0.6201900377869606</v>
       </c>
       <c r="C119" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B120">
-        <v>0.43622211366891861</v>
+        <v>0.4362221136689186</v>
       </c>
       <c r="C120" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B121">
-        <v>0.31711796820163729</v>
+        <v>0.3171179682016373</v>
       </c>
       <c r="C121" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B122">
-        <v>0.59483841694891448</v>
+        <v>0.5948384169489145</v>
       </c>
       <c r="C122" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B123">
-        <v>0.53679392635822298</v>
+        <v>0.536793926358223</v>
       </c>
       <c r="C123" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B124">
-        <v>0.64427864253520961</v>
+        <v>0.6442786425352096</v>
       </c>
       <c r="C124" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B125">
-        <v>0.33887519836425778</v>
+        <v>0.3388751983642578</v>
       </c>
       <c r="C125" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B126">
-        <v>0.65165410637855525</v>
+        <v>0.6516541063785553</v>
       </c>
       <c r="C126" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B127">
         <v>0.3901338793337345</v>
       </c>
       <c r="C127" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B128">
-        <v>0.55399543046951294</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5539954304695129</v>
+      </c>
+      <c r="C128" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B129">
         <v>0.4753774505108595</v>
       </c>
       <c r="C129" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B130">
         <v>0.8050876677036285</v>
       </c>
       <c r="C130" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B131">
-        <v>0.43379222154617308</v>
+        <v>0.4337922215461731</v>
       </c>
       <c r="C131" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B132">
-        <v>0.52498989608138791</v>
+        <v>0.5249898960813879</v>
       </c>
       <c r="C132" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B133">
-        <v>0.46180111933499568</v>
+        <v>0.4618011193349957</v>
       </c>
       <c r="C133" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B134">
-        <v>0.33600407540798188</v>
+        <v>0.3360040754079819</v>
       </c>
       <c r="C134" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B135">
         <v>0.1988454222679138</v>
       </c>
       <c r="C135" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B136">
-        <v>0.52620877437293523</v>
+        <v>0.5262087743729352</v>
       </c>
       <c r="C136" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B137">
         <v>0.5255991659127176</v>
       </c>
       <c r="C137" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B138">
-        <v>0.37800925523042678</v>
+        <v>0.3780092552304268</v>
       </c>
       <c r="C138" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B139">
-        <v>0.84630516171455383</v>
+        <v>0.8463051617145538</v>
       </c>
       <c r="C139" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B140">
         <v>0.8615004360675812</v>
       </c>
       <c r="C140" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B141">
-        <v>0.26851842701435091</v>
+        <v>0.2685184270143509</v>
       </c>
       <c r="C141" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B142">
-        <v>0.36351130604743948</v>
+        <v>0.3635113060474395</v>
       </c>
       <c r="C142" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B143">
-        <v>0.31432822346687322</v>
+        <v>0.3143282234668732</v>
       </c>
       <c r="C143" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B144">
-        <v>0.52769303210079666</v>
+        <v>0.5276930321007967</v>
       </c>
       <c r="C144" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B145">
-        <v>0.49296807739883658</v>
+        <v>0.4929680773988366</v>
       </c>
       <c r="C145" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B146">
-        <v>0.86724809408187864</v>
+        <v>0.8672480940818786</v>
       </c>
       <c r="C146" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B147">
-        <v>0.57685603797435758</v>
+        <v>0.5768560379743576</v>
       </c>
       <c r="C147" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B148">
-        <v>0.33309792280197142</v>
+        <v>0.3330979228019714</v>
       </c>
       <c r="C148" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B149">
-        <v>0.61838717758655548</v>
+        <v>0.6183871775865555</v>
       </c>
       <c r="C149" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B150">
-        <v>0.44674933403730388</v>
+        <v>0.4467493340373039</v>
       </c>
       <c r="C150" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B151">
-        <v>0.36789710819721222</v>
+        <v>0.3678971081972122</v>
       </c>
       <c r="C151" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B152">
-        <v>0.39095488786697391</v>
+        <v>0.3909548878669739</v>
       </c>
       <c r="C152" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B153">
-        <v>0.42705794125795371</v>
+        <v>0.4270579412579537</v>
       </c>
       <c r="C153" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B154">
-        <v>0.46812798902392377</v>
+        <v>0.4681279890239238</v>
       </c>
       <c r="C154" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B155">
-        <v>0.61128862798213957</v>
+        <v>0.6112886279821396</v>
       </c>
       <c r="C155" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B156">
-        <v>0.67534418702125554</v>
+        <v>0.6753441870212555</v>
       </c>
       <c r="C156" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B157">
         <v>0.5380960715934634</v>
       </c>
       <c r="C157" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B158">
-        <v>0.69047741889953618</v>
+        <v>0.6904774188995362</v>
       </c>
       <c r="C158" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B159">
-        <v>0.53520779013633724</v>
+        <v>0.5352077901363372</v>
       </c>
       <c r="C159" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B160">
-        <v>0.29365726411342619</v>
+        <v>0.2936572641134262</v>
       </c>
       <c r="C160" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B161">
-        <v>0.56949418224394321</v>
+        <v>0.5694941822439432</v>
       </c>
       <c r="C161" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B162">
-        <v>0.64427864253520961</v>
+        <v>0.6442786425352096</v>
       </c>
       <c r="C162" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B163">
-        <v>0.59249008297920225</v>
+        <v>0.5924900829792022</v>
       </c>
       <c r="C163" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B164">
-        <v>0.74306082427501674</v>
+        <v>0.7430608242750167</v>
       </c>
       <c r="C164" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B165">
-        <v>0.61320628970861435</v>
+        <v>0.6132062897086143</v>
       </c>
       <c r="C165" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B166">
-        <v>0.47543975412845613</v>
+        <v>0.4754397541284561</v>
       </c>
       <c r="C166" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B167">
-        <v>0.48119206351693722</v>
+        <v>0.4811920635169372</v>
       </c>
       <c r="C167" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B168">
-        <v>0.64488010630011561</v>
+        <v>0.6448801063001156</v>
       </c>
       <c r="C168" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B169">
-        <v>0.31863576173782349</v>
+        <v>0.3186357617378235</v>
       </c>
       <c r="C169" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B170">
         <v>0.9209711372852325</v>
       </c>
       <c r="C170" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B171">
         <v>0.5863680943846703</v>
       </c>
       <c r="C171" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B172">
-        <v>0.67930853664875035</v>
+        <v>0.6793085366487503</v>
       </c>
       <c r="C172" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B173">
-        <v>0.40443549379706378</v>
+        <v>0.4044354937970638</v>
       </c>
       <c r="C173" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B174">
         <v>0.1097570478916168</v>
       </c>
       <c r="C174" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B175">
-        <v>0.46604600064456458</v>
+        <v>0.4660460006445646</v>
       </c>
       <c r="C175" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B176">
-        <v>7.2353780269622803E-2</v>
+        <v>0.0723537802696228</v>
       </c>
       <c r="C176" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B177">
         <v>0.6449042141437531</v>
       </c>
       <c r="C177" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B178">
-        <v>0.43826527297496798</v>
+        <v>0.438265272974968</v>
       </c>
       <c r="C178" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B179">
-        <v>0.59076604396104815</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5907660439610481</v>
+      </c>
+      <c r="C179" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B180">
-        <v>0.58100849948823452</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5810084994882345</v>
+      </c>
+      <c r="C180" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B181">
-        <v>0.58504808060824876</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.5850480806082488</v>
+      </c>
+      <c r="C181" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B182">
-        <v>0.16217772364616401</v>
+        <v>0.162177723646164</v>
       </c>
       <c r="C182" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B183">
-        <v>0.39190486464649438</v>
+        <v>0.3919048646464944</v>
       </c>
       <c r="C183" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B184">
-        <v>0.84758350253105164</v>
+        <v>0.8475835025310516</v>
       </c>
       <c r="C184" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B185">
-        <v>0.88240159153938291</v>
+        <v>0.8824015915393829</v>
       </c>
       <c r="C185" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B186">
-        <v>0.13081600666046139</v>
+        <v>0.1308160066604614</v>
       </c>
       <c r="C186" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B187">
-        <v>0.39113569706678392</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.3911356970667839</v>
+      </c>
+      <c r="C187" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B188">
-        <v>0.76966443657875061</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.7696644365787506</v>
+      </c>
+      <c r="C188" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B189">
-        <v>0.26967472434043882</v>
+        <v>0.2696747243404388</v>
       </c>
       <c r="C189" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B190">
-        <v>0.41315643787384032</v>
+        <v>0.4131564378738403</v>
       </c>
       <c r="C190" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B191">
         <v>0.5042892783880234</v>
       </c>
       <c r="C191" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B192">
-        <v>0.38046959266066549</v>
+        <v>0.3804695926606655</v>
       </c>
       <c r="C192" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B193">
-        <v>0.38910215348005289</v>
+        <v>0.3891021534800529</v>
       </c>
       <c r="C193" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B194">
-        <v>0.48658834211528301</v>
+        <v>0.486588342115283</v>
       </c>
       <c r="C194" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B195">
-        <v>0.45839437600225208</v>
+        <v>0.4583943760022521</v>
       </c>
       <c r="C195" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B196">
         <v>0.4299734652042389</v>
       </c>
       <c r="C196" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B197">
-        <v>0.19076001644134519</v>
+        <v>0.1907600164413452</v>
       </c>
       <c r="C197" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B198">
-        <v>0.55084150359034534</v>
+        <v>0.5508415035903453</v>
       </c>
       <c r="C198" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B199">
-        <v>0.42540581002831462</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.4254058100283146</v>
+      </c>
+      <c r="C199" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B200">
-        <v>0.37078127413988121</v>
+        <v>0.3707812741398812</v>
       </c>
       <c r="C200" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B201">
-        <v>0.39008943885564812</v>
+        <v>0.3900894388556481</v>
       </c>
       <c r="C201" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B202">
-        <v>0.73011186420917507</v>
+        <v>0.7301118642091751</v>
       </c>
       <c r="C202" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B203">
-        <v>0.77884946465492244</v>
+        <v>0.7788494646549224</v>
       </c>
       <c r="C203" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B204">
-        <v>0.75310221314430237</v>
+        <v>0.7531022131443024</v>
       </c>
       <c r="C204" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B205">
-        <v>0.69084853231906895</v>
+        <v>0.690848532319069</v>
       </c>
       <c r="C205" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B206">
-        <v>0.37495374083518979</v>
+        <v>0.3749537408351898</v>
       </c>
       <c r="C206" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B207">
         <v>0.4719191736541688</v>
       </c>
       <c r="C207" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B208">
         <v>0.1266506373882294</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C208" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B209">
-        <v>0.46212865076959131</v>
+        <v>0.4621286507695913</v>
       </c>
       <c r="C209" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B210">
-        <v>0.64671701099723577</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.6467170109972358</v>
+      </c>
+      <c r="C210" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B211">
-        <v>0.35761474967002871</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.3576147496700287</v>
+      </c>
+      <c r="C211" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B212">
-        <v>0.11968096494674681</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+        <v>0.1196809649467468</v>
+      </c>
+      <c r="C212" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B213">
-        <v>0.39180478006601333</v>
+        <v>0.3918047800660133</v>
       </c>
       <c r="C213" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B214">
-        <v>0.24764739274978639</v>
+        <v>0.2476473927497864</v>
       </c>
       <c r="C214" t="s">
-        <v>401</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>